<commit_message>
[Pipette] SCH & PCB update - 1차 완료분
</commit_message>
<xml_diff>
--- a/1_Plasma_Pipette/3_Firmware/Plasma_Gen_MCU_PinMap_20171227.xlsx
+++ b/1_Plasma_Pipette/3_Firmware/Plasma_Gen_MCU_PinMap_20171227.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12975" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12975"/>
   </bookViews>
   <sheets>
     <sheet name="Pin-map V1.0" sheetId="6" r:id="rId1"/>
@@ -16,12 +16,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pin-map V1.0'!$B$15:$T$79</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Pipette V1.0'!$B$15:$O$79</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="353">
   <si>
     <t>Function</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2184,188 +2184,188 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2604,7 +2604,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2639,7 +2639,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2850,7 +2850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M95"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
@@ -2893,10 +2893,10 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="143" t="s">
+      <c r="B3" s="193" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="144"/>
+      <c r="C3" s="194"/>
       <c r="D3" s="2">
         <v>128</v>
       </c>
@@ -2915,10 +2915,10 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="145" t="s">
+      <c r="B4" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="146"/>
+      <c r="C4" s="196"/>
       <c r="D4" s="3">
         <v>16</v>
       </c>
@@ -2938,10 +2938,10 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="145" t="s">
+      <c r="B5" s="195" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="146"/>
+      <c r="C5" s="196"/>
       <c r="D5" s="3">
         <v>48</v>
       </c>
@@ -2963,10 +2963,10 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="145" t="s">
+      <c r="B6" s="195" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="146"/>
+      <c r="C6" s="196"/>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
@@ -2983,10 +2983,10 @@
       <c r="I6" s="15"/>
     </row>
     <row r="7" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="147" t="s">
+      <c r="B7" s="197" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="148"/>
+      <c r="C7" s="198"/>
       <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
@@ -3055,28 +3055,28 @@
     </row>
     <row r="13" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="155" t="s">
+      <c r="B14" s="186" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="149"/>
-      <c r="D14" s="149" t="s">
+      <c r="C14" s="187"/>
+      <c r="D14" s="187" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="149" t="s">
+      <c r="E14" s="187" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="150"/>
-      <c r="G14" s="139" t="s">
+      <c r="F14" s="199"/>
+      <c r="G14" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="140"/>
-      <c r="I14" s="139" t="s">
+      <c r="H14" s="190"/>
+      <c r="I14" s="189" t="s">
         <v>93</v>
       </c>
-      <c r="J14" s="141"/>
-      <c r="K14" s="141"/>
-      <c r="L14" s="141"/>
-      <c r="M14" s="142"/>
+      <c r="J14" s="191"/>
+      <c r="K14" s="191"/>
+      <c r="L14" s="191"/>
+      <c r="M14" s="192"/>
     </row>
     <row r="15" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
@@ -3085,7 +3085,7 @@
       <c r="C15" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="156"/>
+      <c r="D15" s="188"/>
       <c r="E15" s="14" t="s">
         <v>179</v>
       </c>
@@ -3124,10 +3124,10 @@
       <c r="D16" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="151" t="s">
+      <c r="E16" s="182" t="s">
         <v>107</v>
       </c>
-      <c r="F16" s="152"/>
+      <c r="F16" s="183"/>
       <c r="G16" s="41"/>
       <c r="H16" s="96"/>
       <c r="I16" s="110"/>
@@ -3316,10 +3316,10 @@
       <c r="D22" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="E22" s="153" t="s">
+      <c r="E22" s="184" t="s">
         <v>108</v>
       </c>
-      <c r="F22" s="154"/>
+      <c r="F22" s="185"/>
       <c r="G22" s="39" t="s">
         <v>206</v>
       </c>
@@ -3484,10 +3484,10 @@
       <c r="D27" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="E27" s="157" t="s">
+      <c r="E27" s="178" t="s">
         <v>120</v>
       </c>
-      <c r="F27" s="158"/>
+      <c r="F27" s="179"/>
       <c r="G27" s="24"/>
       <c r="H27" s="100"/>
       <c r="I27" s="24"/>
@@ -3506,10 +3506,10 @@
       <c r="D28" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="E28" s="157" t="s">
+      <c r="E28" s="178" t="s">
         <v>121</v>
       </c>
-      <c r="F28" s="158"/>
+      <c r="F28" s="179"/>
       <c r="G28" s="24"/>
       <c r="H28" s="100"/>
       <c r="I28" s="24"/>
@@ -3664,10 +3664,10 @@
       <c r="D33" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="E33" s="157" t="s">
+      <c r="E33" s="178" t="s">
         <v>126</v>
       </c>
-      <c r="F33" s="158"/>
+      <c r="F33" s="179"/>
       <c r="G33" s="24"/>
       <c r="H33" s="100"/>
       <c r="I33" s="24"/>
@@ -3686,10 +3686,10 @@
       <c r="D34" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="E34" s="157" t="s">
+      <c r="E34" s="178" t="s">
         <v>107</v>
       </c>
-      <c r="F34" s="158"/>
+      <c r="F34" s="179"/>
       <c r="G34" s="24"/>
       <c r="H34" s="100"/>
       <c r="I34" s="24"/>
@@ -4086,10 +4086,10 @@
       <c r="D46" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="E46" s="157" t="s">
+      <c r="E46" s="178" t="s">
         <v>126</v>
       </c>
-      <c r="F46" s="158"/>
+      <c r="F46" s="179"/>
       <c r="G46" s="24"/>
       <c r="H46" s="100"/>
       <c r="I46" s="24"/>
@@ -4108,10 +4108,10 @@
       <c r="D47" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="157" t="s">
+      <c r="E47" s="178" t="s">
         <v>107</v>
       </c>
-      <c r="F47" s="158"/>
+      <c r="F47" s="179"/>
       <c r="G47" s="24"/>
       <c r="H47" s="100"/>
       <c r="I47" s="24"/>
@@ -4616,10 +4616,10 @@
       <c r="D62" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="E62" s="157" t="s">
+      <c r="E62" s="178" t="s">
         <v>126</v>
       </c>
-      <c r="F62" s="158"/>
+      <c r="F62" s="179"/>
       <c r="G62" s="24"/>
       <c r="H62" s="100"/>
       <c r="I62" s="24"/>
@@ -4638,10 +4638,10 @@
       <c r="D63" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="E63" s="157" t="s">
+      <c r="E63" s="178" t="s">
         <v>107</v>
       </c>
-      <c r="F63" s="158"/>
+      <c r="F63" s="179"/>
       <c r="G63" s="24"/>
       <c r="H63" s="100"/>
       <c r="I63" s="24"/>
@@ -5034,10 +5034,10 @@
       <c r="D75" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="E75" s="157" t="s">
+      <c r="E75" s="178" t="s">
         <v>175</v>
       </c>
-      <c r="F75" s="158"/>
+      <c r="F75" s="179"/>
       <c r="G75" s="24" t="s">
         <v>224</v>
       </c>
@@ -5134,10 +5134,10 @@
       <c r="D78" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="E78" s="157" t="s">
+      <c r="E78" s="178" t="s">
         <v>126</v>
       </c>
-      <c r="F78" s="158"/>
+      <c r="F78" s="179"/>
       <c r="G78" s="24"/>
       <c r="H78" s="100"/>
       <c r="I78" s="24"/>
@@ -5156,10 +5156,10 @@
       <c r="D79" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="E79" s="159" t="s">
+      <c r="E79" s="180" t="s">
         <v>107</v>
       </c>
-      <c r="F79" s="160"/>
+      <c r="F79" s="181"/>
       <c r="G79" s="25"/>
       <c r="H79" s="106"/>
       <c r="I79" s="25"/>
@@ -5219,21 +5219,6 @@
   </sheetData>
   <autoFilter ref="B15:T79"/>
   <mergeCells count="23">
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E27:F27"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="I14:M14"/>
     <mergeCell ref="B3:C3"/>
@@ -5242,6 +5227,21 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="E75:F75"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5253,8 +5253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42:K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5293,10 +5293,10 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="143" t="s">
+      <c r="B3" s="193" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="144"/>
+      <c r="C3" s="194"/>
       <c r="D3" s="2">
         <v>128</v>
       </c>
@@ -5315,10 +5315,10 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="145" t="s">
+      <c r="B4" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="146"/>
+      <c r="C4" s="196"/>
       <c r="D4" s="3">
         <v>16</v>
       </c>
@@ -5338,10 +5338,10 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="145" t="s">
+      <c r="B5" s="195" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="146"/>
+      <c r="C5" s="196"/>
       <c r="D5" s="3">
         <v>48</v>
       </c>
@@ -5363,10 +5363,10 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="145" t="s">
+      <c r="B6" s="195" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="146"/>
+      <c r="C6" s="196"/>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
@@ -5383,10 +5383,10 @@
       <c r="I6" s="15"/>
     </row>
     <row r="7" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="147" t="s">
+      <c r="B7" s="197" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="148"/>
+      <c r="C7" s="198"/>
       <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
@@ -5455,28 +5455,28 @@
     </row>
     <row r="13" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="155" t="s">
+      <c r="B14" s="186" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="149"/>
-      <c r="D14" s="149" t="s">
+      <c r="C14" s="187"/>
+      <c r="D14" s="187" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="149" t="s">
+      <c r="E14" s="187" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="150"/>
-      <c r="G14" s="139" t="s">
+      <c r="F14" s="199"/>
+      <c r="G14" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="140"/>
-      <c r="I14" s="139" t="s">
+      <c r="H14" s="190"/>
+      <c r="I14" s="189" t="s">
         <v>315</v>
       </c>
-      <c r="J14" s="141"/>
-      <c r="K14" s="141"/>
-      <c r="L14" s="141"/>
-      <c r="M14" s="142"/>
+      <c r="J14" s="191"/>
+      <c r="K14" s="191"/>
+      <c r="L14" s="191"/>
+      <c r="M14" s="192"/>
     </row>
     <row r="15" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
@@ -5485,7 +5485,7 @@
       <c r="C15" s="136" t="s">
         <v>317</v>
       </c>
-      <c r="D15" s="156"/>
+      <c r="D15" s="188"/>
       <c r="E15" s="94" t="s">
         <v>179</v>
       </c>
@@ -5524,10 +5524,10 @@
       <c r="D16" s="91" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="151" t="s">
+      <c r="E16" s="182" t="s">
         <v>107</v>
       </c>
-      <c r="F16" s="152"/>
+      <c r="F16" s="183"/>
       <c r="G16" s="41"/>
       <c r="H16" s="96"/>
       <c r="I16" s="110"/>
@@ -5716,20 +5716,20 @@
       <c r="D22" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="E22" s="153" t="s">
+      <c r="E22" s="184" t="s">
         <v>108</v>
       </c>
-      <c r="F22" s="154"/>
+      <c r="F22" s="185"/>
       <c r="G22" s="84" t="s">
         <v>101</v>
       </c>
-      <c r="H22" s="170" t="s">
-        <v>40</v>
-      </c>
-      <c r="I22" s="181" t="s">
+      <c r="H22" s="149" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="160" t="s">
         <v>101</v>
       </c>
-      <c r="J22" s="174" t="s">
+      <c r="J22" s="153" t="s">
         <v>185</v>
       </c>
       <c r="K22" s="44" t="s">
@@ -5776,7 +5776,7 @@
       <c r="B24" s="114">
         <v>9</v>
       </c>
-      <c r="C24" s="192" t="s">
+      <c r="C24" s="171" t="s">
         <v>322</v>
       </c>
       <c r="D24" s="20" t="s">
@@ -5794,10 +5794,10 @@
       <c r="H24" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="I24" s="181" t="s">
+      <c r="I24" s="160" t="s">
         <v>325</v>
       </c>
-      <c r="J24" s="174" t="s">
+      <c r="J24" s="153" t="s">
         <v>195</v>
       </c>
       <c r="K24" s="44" t="s">
@@ -5810,7 +5810,7 @@
       <c r="B25" s="114">
         <v>10</v>
       </c>
-      <c r="C25" s="192" t="s">
+      <c r="C25" s="171" t="s">
         <v>322</v>
       </c>
       <c r="D25" s="20" t="s">
@@ -5828,10 +5828,10 @@
       <c r="H25" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="I25" s="181" t="s">
+      <c r="I25" s="160" t="s">
         <v>326</v>
       </c>
-      <c r="J25" s="174" t="s">
+      <c r="J25" s="153" t="s">
         <v>193</v>
       </c>
       <c r="K25" s="44" t="s">
@@ -5844,7 +5844,7 @@
       <c r="B26" s="114">
         <v>11</v>
       </c>
-      <c r="C26" s="192" t="s">
+      <c r="C26" s="171" t="s">
         <v>322</v>
       </c>
       <c r="D26" s="20" t="s">
@@ -5862,10 +5862,10 @@
       <c r="H26" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="I26" s="181" t="s">
+      <c r="I26" s="160" t="s">
         <v>327</v>
       </c>
-      <c r="J26" s="174" t="s">
+      <c r="J26" s="153" t="s">
         <v>328</v>
       </c>
       <c r="K26" s="44" t="s">
@@ -5884,10 +5884,10 @@
       <c r="D27" s="89" t="s">
         <v>118</v>
       </c>
-      <c r="E27" s="157" t="s">
+      <c r="E27" s="178" t="s">
         <v>120</v>
       </c>
-      <c r="F27" s="158"/>
+      <c r="F27" s="179"/>
       <c r="G27" s="24"/>
       <c r="H27" s="100"/>
       <c r="I27" s="24"/>
@@ -5906,10 +5906,10 @@
       <c r="D28" s="89" t="s">
         <v>119</v>
       </c>
-      <c r="E28" s="157" t="s">
+      <c r="E28" s="178" t="s">
         <v>121</v>
       </c>
-      <c r="F28" s="158"/>
+      <c r="F28" s="179"/>
       <c r="G28" s="24"/>
       <c r="H28" s="100"/>
       <c r="I28" s="24"/>
@@ -5956,7 +5956,7 @@
       <c r="B30" s="114">
         <v>15</v>
       </c>
-      <c r="C30" s="192" t="s">
+      <c r="C30" s="171" t="s">
         <v>322</v>
       </c>
       <c r="D30" s="20" t="s">
@@ -5974,10 +5974,10 @@
       <c r="H30" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="I30" s="182" t="s">
+      <c r="I30" s="161" t="s">
         <v>347</v>
       </c>
-      <c r="J30" s="175" t="s">
+      <c r="J30" s="154" t="s">
         <v>311</v>
       </c>
       <c r="K30" s="82" t="s">
@@ -5990,7 +5990,7 @@
       <c r="B31" s="114">
         <v>16</v>
       </c>
-      <c r="C31" s="192" t="s">
+      <c r="C31" s="171" t="s">
         <v>322</v>
       </c>
       <c r="D31" s="20" t="s">
@@ -6008,10 +6008,10 @@
       <c r="H31" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="I31" s="182" t="s">
+      <c r="I31" s="161" t="s">
         <v>348</v>
       </c>
-      <c r="J31" s="175" t="s">
+      <c r="J31" s="154" t="s">
         <v>311</v>
       </c>
       <c r="K31" s="82" t="s">
@@ -6064,10 +6064,10 @@
       <c r="D33" s="89" t="s">
         <v>150</v>
       </c>
-      <c r="E33" s="157" t="s">
+      <c r="E33" s="178" t="s">
         <v>126</v>
       </c>
-      <c r="F33" s="158"/>
+      <c r="F33" s="179"/>
       <c r="G33" s="24"/>
       <c r="H33" s="100"/>
       <c r="I33" s="24"/>
@@ -6086,10 +6086,10 @@
       <c r="D34" s="89" t="s">
         <v>95</v>
       </c>
-      <c r="E34" s="157" t="s">
+      <c r="E34" s="178" t="s">
         <v>107</v>
       </c>
-      <c r="F34" s="158"/>
+      <c r="F34" s="179"/>
       <c r="G34" s="24"/>
       <c r="H34" s="100"/>
       <c r="I34" s="24"/>
@@ -6201,13 +6201,13 @@
       <c r="M37" s="15"/>
     </row>
     <row r="38" spans="2:13" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B38" s="196">
+      <c r="B38" s="174">
         <v>23</v>
       </c>
-      <c r="C38" s="197" t="s">
+      <c r="C38" s="175" t="s">
         <v>322</v>
       </c>
-      <c r="D38" s="198" t="s">
+      <c r="D38" s="176" t="s">
         <v>68</v>
       </c>
       <c r="E38" s="10" t="s">
@@ -6216,32 +6216,32 @@
       <c r="F38" s="93" t="s">
         <v>330</v>
       </c>
-      <c r="G38" s="173" t="s">
+      <c r="G38" s="152" t="s">
         <v>330</v>
       </c>
-      <c r="H38" s="165" t="s">
+      <c r="H38" s="144" t="s">
         <v>332</v>
       </c>
-      <c r="I38" s="183" t="s">
+      <c r="I38" s="162" t="s">
         <v>350</v>
       </c>
-      <c r="J38" s="176" t="s">
+      <c r="J38" s="155" t="s">
         <v>202</v>
       </c>
-      <c r="K38" s="161" t="s">
+      <c r="K38" s="140" t="s">
         <v>40</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="15"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B39" s="196">
+      <c r="B39" s="174">
         <v>24</v>
       </c>
-      <c r="C39" s="197" t="s">
+      <c r="C39" s="175" t="s">
         <v>322</v>
       </c>
-      <c r="D39" s="198" t="s">
+      <c r="D39" s="176" t="s">
         <v>69</v>
       </c>
       <c r="E39" s="92" t="s">
@@ -6250,19 +6250,19 @@
       <c r="F39" s="93" t="s">
         <v>331</v>
       </c>
-      <c r="G39" s="173" t="s">
+      <c r="G39" s="152" t="s">
         <v>331</v>
       </c>
-      <c r="H39" s="165" t="s">
+      <c r="H39" s="144" t="s">
         <v>332</v>
       </c>
-      <c r="I39" s="183" t="s">
+      <c r="I39" s="162" t="s">
         <v>351</v>
       </c>
-      <c r="J39" s="176" t="s">
+      <c r="J39" s="155" t="s">
         <v>202</v>
       </c>
-      <c r="K39" s="161" t="s">
+      <c r="K39" s="140" t="s">
         <v>40</v>
       </c>
       <c r="L39" s="3"/>
@@ -6272,7 +6272,7 @@
       <c r="B40" s="114">
         <v>25</v>
       </c>
-      <c r="C40" s="192" t="s">
+      <c r="C40" s="171" t="s">
         <v>322</v>
       </c>
       <c r="D40" s="20" t="s">
@@ -6290,16 +6290,16 @@
       <c r="H40" s="99" t="s">
         <v>332</v>
       </c>
-      <c r="I40" s="182" t="s">
+      <c r="I40" s="161" t="s">
         <v>349</v>
       </c>
-      <c r="J40" s="175" t="s">
+      <c r="J40" s="154" t="s">
         <v>316</v>
       </c>
       <c r="K40" s="82" t="s">
         <v>189</v>
       </c>
-      <c r="L40" s="166"/>
+      <c r="L40" s="145"/>
       <c r="M40" s="15" t="s">
         <v>239</v>
       </c>
@@ -6308,7 +6308,7 @@
       <c r="B41" s="114">
         <v>26</v>
       </c>
-      <c r="C41" s="192" t="s">
+      <c r="C41" s="171" t="s">
         <v>322</v>
       </c>
       <c r="D41" s="20" t="s">
@@ -6326,23 +6326,23 @@
       <c r="H41" s="99" t="s">
         <v>332</v>
       </c>
-      <c r="I41" s="181" t="s">
+      <c r="I41" s="160" t="s">
         <v>187</v>
       </c>
-      <c r="J41" s="174" t="s">
+      <c r="J41" s="153" t="s">
         <v>197</v>
       </c>
       <c r="K41" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="L41" s="166"/>
+      <c r="L41" s="145"/>
       <c r="M41" s="15"/>
     </row>
     <row r="42" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B42" s="114">
         <v>27</v>
       </c>
-      <c r="C42" s="192" t="s">
+      <c r="C42" s="171" t="s">
         <v>322</v>
       </c>
       <c r="D42" s="20" t="s">
@@ -6360,16 +6360,16 @@
       <c r="H42" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="I42" s="182" t="s">
+      <c r="I42" s="161" t="s">
         <v>313</v>
       </c>
-      <c r="J42" s="175" t="s">
+      <c r="J42" s="154" t="s">
         <v>219</v>
       </c>
       <c r="K42" s="125" t="s">
         <v>40</v>
       </c>
-      <c r="L42" s="167" t="s">
+      <c r="L42" s="146" t="s">
         <v>314</v>
       </c>
       <c r="M42" s="122"/>
@@ -6390,23 +6390,6 @@
       <c r="F43" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G43" s="130" t="s">
-        <v>19</v>
-      </c>
-      <c r="H43" s="99" t="s">
-        <v>332</v>
-      </c>
-      <c r="I43" s="199" t="s">
-        <v>333</v>
-      </c>
-      <c r="J43" s="177" t="s">
-        <v>336</v>
-      </c>
-      <c r="K43" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="L43" s="166"/>
-      <c r="M43" s="15"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B44" s="114">
@@ -6424,23 +6407,6 @@
       <c r="F44" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G44" s="130" t="s">
-        <v>19</v>
-      </c>
-      <c r="H44" s="99" t="s">
-        <v>332</v>
-      </c>
-      <c r="I44" s="199" t="s">
-        <v>334</v>
-      </c>
-      <c r="J44" s="177" t="s">
-        <v>337</v>
-      </c>
-      <c r="K44" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="L44" s="166"/>
-      <c r="M44" s="15"/>
     </row>
     <row r="45" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B45" s="114">
@@ -6458,23 +6424,6 @@
       <c r="F45" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G45" s="130" t="s">
-        <v>19</v>
-      </c>
-      <c r="H45" s="99" t="s">
-        <v>332</v>
-      </c>
-      <c r="I45" s="199" t="s">
-        <v>335</v>
-      </c>
-      <c r="J45" s="177" t="s">
-        <v>338</v>
-      </c>
-      <c r="K45" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="L45" s="166"/>
-      <c r="M45" s="15"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B46" s="24">
@@ -6486,16 +6435,16 @@
       <c r="D46" s="89" t="s">
         <v>150</v>
       </c>
-      <c r="E46" s="157" t="s">
+      <c r="E46" s="178" t="s">
         <v>126</v>
       </c>
-      <c r="F46" s="158"/>
+      <c r="F46" s="179"/>
       <c r="G46" s="24"/>
       <c r="H46" s="100"/>
       <c r="I46" s="24"/>
       <c r="J46" s="89"/>
       <c r="K46" s="89"/>
-      <c r="L46" s="166"/>
+      <c r="L46" s="145"/>
       <c r="M46" s="15"/>
     </row>
     <row r="47" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -6508,23 +6457,23 @@
       <c r="D47" s="89" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="157" t="s">
+      <c r="E47" s="178" t="s">
         <v>107</v>
       </c>
-      <c r="F47" s="158"/>
+      <c r="F47" s="179"/>
       <c r="G47" s="24"/>
       <c r="H47" s="100"/>
       <c r="I47" s="24"/>
       <c r="J47" s="89"/>
       <c r="K47" s="89"/>
-      <c r="L47" s="166"/>
+      <c r="L47" s="145"/>
       <c r="M47" s="15"/>
     </row>
     <row r="48" spans="2:13" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B48" s="114">
         <v>33</v>
       </c>
-      <c r="C48" s="193" t="s">
+      <c r="C48" s="172" t="s">
         <v>320</v>
       </c>
       <c r="D48" s="20" t="s">
@@ -6542,16 +6491,16 @@
       <c r="H48" s="99" t="s">
         <v>222</v>
       </c>
-      <c r="I48" s="181" t="s">
+      <c r="I48" s="160" t="s">
         <v>223</v>
       </c>
-      <c r="J48" s="174" t="s">
+      <c r="J48" s="153" t="s">
         <v>219</v>
       </c>
       <c r="K48" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="L48" s="168"/>
+      <c r="L48" s="147"/>
       <c r="M48" s="15" t="s">
         <v>237</v>
       </c>
@@ -6578,16 +6527,16 @@
       <c r="H49" s="99" t="s">
         <v>222</v>
       </c>
-      <c r="I49" s="184" t="s">
+      <c r="I49" s="163" t="s">
         <v>339</v>
       </c>
-      <c r="J49" s="177" t="s">
+      <c r="J49" s="156" t="s">
         <v>340</v>
       </c>
       <c r="K49" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="L49" s="166"/>
+      <c r="L49" s="145"/>
       <c r="M49" s="15"/>
     </row>
     <row r="50" spans="2:13" ht="49.5" x14ac:dyDescent="0.3">
@@ -6606,22 +6555,22 @@
       <c r="F50" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G50" s="23" t="s">
-        <v>305</v>
-      </c>
-      <c r="H50" s="97" t="s">
-        <v>306</v>
-      </c>
-      <c r="I50" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="J50" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="K50" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L50" s="166"/>
+      <c r="G50" s="130" t="s">
+        <v>19</v>
+      </c>
+      <c r="H50" s="99" t="s">
+        <v>332</v>
+      </c>
+      <c r="I50" s="177" t="s">
+        <v>335</v>
+      </c>
+      <c r="J50" s="156" t="s">
+        <v>338</v>
+      </c>
+      <c r="K50" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="L50" s="145"/>
       <c r="M50" s="15"/>
     </row>
     <row r="51" spans="2:13" ht="33" x14ac:dyDescent="0.3">
@@ -6640,27 +6589,23 @@
       <c r="F51" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="G51" s="84" t="s">
-        <v>204</v>
+      <c r="G51" s="130" t="s">
+        <v>19</v>
       </c>
       <c r="H51" s="99" t="s">
-        <v>20</v>
-      </c>
-      <c r="I51" s="181" t="s">
-        <v>218</v>
-      </c>
-      <c r="J51" s="174" t="s">
-        <v>201</v>
+        <v>332</v>
+      </c>
+      <c r="I51" s="177" t="s">
+        <v>334</v>
+      </c>
+      <c r="J51" s="156" t="s">
+        <v>337</v>
       </c>
       <c r="K51" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="L51" s="168" t="s">
-        <v>233</v>
-      </c>
-      <c r="M51" s="15" t="s">
-        <v>238</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="L51" s="145"/>
+      <c r="M51" s="15"/>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B52" s="22">
@@ -6678,22 +6623,22 @@
       <c r="F52" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G52" s="23" t="s">
-        <v>305</v>
-      </c>
-      <c r="H52" s="97" t="s">
-        <v>306</v>
-      </c>
-      <c r="I52" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="J52" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="K52" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L52" s="3"/>
+      <c r="G52" s="130" t="s">
+        <v>19</v>
+      </c>
+      <c r="H52" s="99" t="s">
+        <v>332</v>
+      </c>
+      <c r="I52" s="177" t="s">
+        <v>333</v>
+      </c>
+      <c r="J52" s="156" t="s">
+        <v>336</v>
+      </c>
+      <c r="K52" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="L52" s="145"/>
       <c r="M52" s="15"/>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.3">
@@ -6718,16 +6663,16 @@
       <c r="H53" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="I53" s="182" t="s">
+      <c r="I53" s="161" t="s">
         <v>243</v>
       </c>
-      <c r="J53" s="175" t="s">
+      <c r="J53" s="154" t="s">
         <v>201</v>
       </c>
       <c r="K53" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="L53" s="172" t="s">
+      <c r="L53" s="151" t="s">
         <v>241</v>
       </c>
       <c r="M53" s="15" t="s">
@@ -6803,7 +6748,7 @@
       <c r="M55" s="15"/>
     </row>
     <row r="56" spans="2:13" ht="33" x14ac:dyDescent="0.3">
-      <c r="B56" s="194">
+      <c r="B56" s="173">
         <v>41</v>
       </c>
       <c r="C56" s="86" t="s">
@@ -6824,10 +6769,10 @@
       <c r="H56" s="101" t="s">
         <v>309</v>
       </c>
-      <c r="I56" s="185" t="s">
+      <c r="I56" s="164" t="s">
         <v>216</v>
       </c>
-      <c r="J56" s="178" t="s">
+      <c r="J56" s="157" t="s">
         <v>215</v>
       </c>
       <c r="K56" s="86" t="s">
@@ -6840,7 +6785,7 @@
       <c r="B57" s="50">
         <v>42</v>
       </c>
-      <c r="C57" s="162" t="s">
+      <c r="C57" s="141" t="s">
         <v>320</v>
       </c>
       <c r="D57" s="47" t="s">
@@ -6858,10 +6803,10 @@
       <c r="H57" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="I57" s="186" t="s">
+      <c r="I57" s="165" t="s">
         <v>352</v>
       </c>
-      <c r="J57" s="179" t="s">
+      <c r="J57" s="158" t="s">
         <v>200</v>
       </c>
       <c r="K57" s="53" t="s">
@@ -6874,7 +6819,7 @@
       <c r="B58" s="50">
         <v>43</v>
       </c>
-      <c r="C58" s="162" t="s">
+      <c r="C58" s="141" t="s">
         <v>320</v>
       </c>
       <c r="D58" s="47" t="s">
@@ -6892,10 +6837,10 @@
       <c r="H58" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="I58" s="186" t="s">
+      <c r="I58" s="165" t="s">
         <v>210</v>
       </c>
-      <c r="J58" s="179" t="s">
+      <c r="J58" s="158" t="s">
         <v>200</v>
       </c>
       <c r="K58" s="53" t="s">
@@ -6905,7 +6850,7 @@
       <c r="M58" s="15"/>
     </row>
     <row r="59" spans="2:13" ht="33" x14ac:dyDescent="0.3">
-      <c r="B59" s="194">
+      <c r="B59" s="173">
         <v>44</v>
       </c>
       <c r="C59" s="86" t="s">
@@ -6926,10 +6871,10 @@
       <c r="H59" s="101" t="s">
         <v>309</v>
       </c>
-      <c r="I59" s="185" t="s">
+      <c r="I59" s="164" t="s">
         <v>217</v>
       </c>
-      <c r="J59" s="178" t="s">
+      <c r="J59" s="157" t="s">
         <v>215</v>
       </c>
       <c r="K59" s="86" t="s">
@@ -6960,10 +6905,10 @@
       <c r="H60" s="99" t="s">
         <v>222</v>
       </c>
-      <c r="I60" s="181" t="s">
+      <c r="I60" s="160" t="s">
         <v>208</v>
       </c>
-      <c r="J60" s="174" t="s">
+      <c r="J60" s="153" t="s">
         <v>181</v>
       </c>
       <c r="K60" s="44" t="s">
@@ -6976,7 +6921,7 @@
       <c r="B61" s="57">
         <v>46</v>
       </c>
-      <c r="C61" s="163" t="s">
+      <c r="C61" s="142" t="s">
         <v>320</v>
       </c>
       <c r="D61" s="54" t="s">
@@ -6988,19 +6933,19 @@
       <c r="F61" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="G61" s="188" t="s">
+      <c r="G61" s="167" t="s">
         <v>61</v>
       </c>
-      <c r="H61" s="189" t="s">
+      <c r="H61" s="168" t="s">
         <v>58</v>
       </c>
-      <c r="I61" s="190" t="s">
+      <c r="I61" s="169" t="s">
         <v>61</v>
       </c>
-      <c r="J61" s="191" t="s">
+      <c r="J61" s="170" t="s">
         <v>59</v>
       </c>
-      <c r="K61" s="164" t="s">
+      <c r="K61" s="143" t="s">
         <v>199</v>
       </c>
       <c r="L61" s="3"/>
@@ -7016,10 +6961,10 @@
       <c r="D62" s="89" t="s">
         <v>150</v>
       </c>
-      <c r="E62" s="157" t="s">
+      <c r="E62" s="178" t="s">
         <v>126</v>
       </c>
-      <c r="F62" s="158"/>
+      <c r="F62" s="179"/>
       <c r="G62" s="24"/>
       <c r="H62" s="100"/>
       <c r="I62" s="24"/>
@@ -7028,20 +6973,20 @@
       <c r="L62" s="3"/>
       <c r="M62" s="15"/>
     </row>
-    <row r="63" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B63" s="24">
         <v>48</v>
       </c>
-      <c r="C63" s="127" t="s">
+      <c r="C63" s="139" t="s">
         <v>318</v>
       </c>
-      <c r="D63" s="89" t="s">
+      <c r="D63" s="139" t="s">
         <v>95</v>
       </c>
-      <c r="E63" s="157" t="s">
+      <c r="E63" s="178" t="s">
         <v>107</v>
       </c>
-      <c r="F63" s="158"/>
+      <c r="F63" s="179"/>
       <c r="G63" s="24"/>
       <c r="H63" s="100"/>
       <c r="I63" s="24"/>
@@ -7054,7 +6999,7 @@
       <c r="B64" s="57">
         <v>49</v>
       </c>
-      <c r="C64" s="195" t="s">
+      <c r="C64" s="142" t="s">
         <v>320</v>
       </c>
       <c r="D64" s="54" t="s">
@@ -7066,19 +7011,19 @@
       <c r="F64" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="G64" s="188" t="s">
+      <c r="G64" s="167" t="s">
         <v>57</v>
       </c>
-      <c r="H64" s="189" t="s">
+      <c r="H64" s="168" t="s">
         <v>58</v>
       </c>
-      <c r="I64" s="190" t="s">
+      <c r="I64" s="169" t="s">
         <v>57</v>
       </c>
-      <c r="J64" s="191" t="s">
+      <c r="J64" s="170" t="s">
         <v>59</v>
       </c>
-      <c r="K64" s="164" t="s">
+      <c r="K64" s="143" t="s">
         <v>198</v>
       </c>
       <c r="L64" s="3"/>
@@ -7100,23 +7045,27 @@
       <c r="F65" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G65" s="23" t="s">
-        <v>305</v>
-      </c>
-      <c r="H65" s="97" t="s">
-        <v>306</v>
-      </c>
-      <c r="I65" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="J65" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="K65" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L65" s="3"/>
-      <c r="M65" s="15"/>
+      <c r="G65" s="84" t="s">
+        <v>204</v>
+      </c>
+      <c r="H65" s="99" t="s">
+        <v>20</v>
+      </c>
+      <c r="I65" s="160" t="s">
+        <v>218</v>
+      </c>
+      <c r="J65" s="153" t="s">
+        <v>201</v>
+      </c>
+      <c r="K65" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="L65" s="147" t="s">
+        <v>233</v>
+      </c>
+      <c r="M65" s="15" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B66" s="22">
@@ -7310,10 +7259,10 @@
       <c r="H71" s="99" t="s">
         <v>329</v>
       </c>
-      <c r="I71" s="184" t="s">
+      <c r="I71" s="163" t="s">
         <v>342</v>
       </c>
-      <c r="J71" s="177" t="s">
+      <c r="J71" s="156" t="s">
         <v>344</v>
       </c>
       <c r="K71" s="88" t="s">
@@ -7380,10 +7329,10 @@
       <c r="H73" s="99" t="s">
         <v>329</v>
       </c>
-      <c r="I73" s="184" t="s">
+      <c r="I73" s="163" t="s">
         <v>343</v>
       </c>
-      <c r="J73" s="177" t="s">
+      <c r="J73" s="156" t="s">
         <v>344</v>
       </c>
       <c r="K73" s="88" t="s">
@@ -7425,7 +7374,7 @@
       <c r="K74" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="L74" s="166"/>
+      <c r="L74" s="145"/>
       <c r="M74" s="15"/>
     </row>
     <row r="75" spans="2:13" x14ac:dyDescent="0.3">
@@ -7438,20 +7387,20 @@
       <c r="D75" s="89" t="s">
         <v>156</v>
       </c>
-      <c r="E75" s="157" t="s">
+      <c r="E75" s="178" t="s">
         <v>175</v>
       </c>
-      <c r="F75" s="158"/>
+      <c r="F75" s="179"/>
       <c r="G75" s="24" t="s">
         <v>224</v>
       </c>
       <c r="H75" s="100"/>
-      <c r="I75" s="187" t="s">
+      <c r="I75" s="166" t="s">
         <v>224</v>
       </c>
-      <c r="J75" s="180"/>
+      <c r="J75" s="159"/>
       <c r="K75" s="89"/>
-      <c r="L75" s="166"/>
+      <c r="L75" s="145"/>
       <c r="M75" s="15"/>
     </row>
     <row r="76" spans="2:13" x14ac:dyDescent="0.3">
@@ -7476,10 +7425,10 @@
       <c r="H76" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="I76" s="181" t="s">
+      <c r="I76" s="160" t="s">
         <v>234</v>
       </c>
-      <c r="J76" s="174" t="s">
+      <c r="J76" s="153" t="s">
         <v>214</v>
       </c>
       <c r="K76" s="44" t="s">
@@ -7514,16 +7463,16 @@
       <c r="H77" s="99" t="s">
         <v>329</v>
       </c>
-      <c r="I77" s="181" t="s">
+      <c r="I77" s="160" t="s">
         <v>207</v>
       </c>
-      <c r="J77" s="174" t="s">
+      <c r="J77" s="153" t="s">
         <v>228</v>
       </c>
       <c r="K77" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="L77" s="168"/>
+      <c r="L77" s="147"/>
       <c r="M77" s="15" t="s">
         <v>235</v>
       </c>
@@ -7538,10 +7487,10 @@
       <c r="D78" s="89" t="s">
         <v>150</v>
       </c>
-      <c r="E78" s="157" t="s">
+      <c r="E78" s="178" t="s">
         <v>126</v>
       </c>
-      <c r="F78" s="158"/>
+      <c r="F78" s="179"/>
       <c r="G78" s="24"/>
       <c r="H78" s="100"/>
       <c r="I78" s="24"/>
@@ -7560,10 +7509,10 @@
       <c r="D79" s="90" t="s">
         <v>95</v>
       </c>
-      <c r="E79" s="159" t="s">
+      <c r="E79" s="180" t="s">
         <v>107</v>
       </c>
-      <c r="F79" s="160"/>
+      <c r="F79" s="181"/>
       <c r="G79" s="25"/>
       <c r="H79" s="106"/>
       <c r="I79" s="25"/>
@@ -7589,7 +7538,7 @@
       <c r="H86" s="99" t="s">
         <v>329</v>
       </c>
-      <c r="I86" s="171" t="s">
+      <c r="I86" s="150" t="s">
         <v>342</v>
       </c>
       <c r="J86" s="88" t="s">
@@ -7611,7 +7560,7 @@
       <c r="I87" s="118" t="s">
         <v>196</v>
       </c>
-      <c r="J87" s="169" t="s">
+      <c r="J87" s="148" t="s">
         <v>316</v>
       </c>
       <c r="K87" s="82" t="s">
@@ -7627,7 +7576,7 @@
       <c r="H88" s="99" t="s">
         <v>329</v>
       </c>
-      <c r="I88" s="171" t="s">
+      <c r="I88" s="150" t="s">
         <v>343</v>
       </c>
       <c r="J88" s="88" t="s">
@@ -7698,6 +7647,17 @@
   </sheetData>
   <autoFilter ref="B15:O79"/>
   <mergeCells count="23">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E22:F22"/>
     <mergeCell ref="E79:F79"/>
     <mergeCell ref="I14:M14"/>
     <mergeCell ref="E62:F62"/>
@@ -7706,21 +7666,10 @@
     <mergeCell ref="E78:F78"/>
     <mergeCell ref="E46:F46"/>
     <mergeCell ref="E47:F47"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E22:F22"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>